<commit_message>
Adding color to boxes and changing labels of boxes
</commit_message>
<xml_diff>
--- a/app/uploads/ucsd12.xlsx
+++ b/app/uploads/ucsd12.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucsdhs-my.sharepoint.com/personal/rrutvik_health_ucsd_edu/Documents/Personalized MH/MH Results/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE933956-6357-4308-A34D-35CA5E6E7D64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="114_{327975AA-3153-6445-9485-5A14BF031625}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{961AEC6F-8917-49A4-A148-0FE355995562}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="16100" windowHeight="9660" firstSheet="6" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="rf" sheetId="1" r:id="rId1"/>
-    <sheet name="gb" sheetId="2" r:id="rId2"/>
-    <sheet name="ab" sheetId="3" r:id="rId3"/>
-    <sheet name="rfb" sheetId="4" r:id="rId4"/>
-    <sheet name="models" sheetId="5" r:id="rId5"/>
-    <sheet name="best_model(gb)" sheetId="6" r:id="rId6"/>
+    <sheet name="best_model(gb)" sheetId="6" r:id="rId1"/>
+    <sheet name="rf" sheetId="1" r:id="rId2"/>
+    <sheet name="gb" sheetId="2" r:id="rId3"/>
+    <sheet name="ab" sheetId="3" r:id="rId4"/>
+    <sheet name="rfb" sheetId="4" r:id="rId5"/>
+    <sheet name="models" sheetId="5" r:id="rId6"/>
     <sheet name="weekly_summary" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -59,6 +59,303 @@
     <t>MannWhitneyUTest_pval</t>
   </si>
   <si>
+    <t>rank</t>
+  </si>
+  <si>
+    <t>prev_night_sleep</t>
+  </si>
+  <si>
+    <t>{0: 5.184126347678875, 1: 5.792857142857143}</t>
+  </si>
+  <si>
+    <t>{0: 2.5056831230876324, 1: 2.7848008896716467}</t>
+  </si>
+  <si>
+    <t>{0: 5.366666666666666, 1: 6.433333333333334}</t>
+  </si>
+  <si>
+    <t>{0: 1.7544100000000002, 1: 4.991420000000001}</t>
+  </si>
+  <si>
+    <t>ppg_std</t>
+  </si>
+  <si>
+    <t>{0: 144895.1541374223, 1: 180694.1595503829}</t>
+  </si>
+  <si>
+    <t>{0: 132374.97157583816, 1: 107879.52708056483}</t>
+  </si>
+  <si>
+    <t>{0: 95494.37235792716, 1: 151613.34293190698}</t>
+  </si>
+  <si>
+    <t>{0: 71328.03351750519, 1: 113676.25562711658}</t>
+  </si>
+  <si>
+    <t>cumm_step_distance</t>
+  </si>
+  <si>
+    <t>{0: 2126.4325836626754, 1: 994.6574599785714}</t>
+  </si>
+  <si>
+    <t>{0: 2250.126647830915, 1: 1289.388057974536}</t>
+  </si>
+  <si>
+    <t>{0: 1535.981761385, 1: 464.135351065}</t>
+  </si>
+  <si>
+    <t>{0: 2081.1825957916767, 1: 343.5841717532699}</t>
+  </si>
+  <si>
+    <t>cumm_step_speed</t>
+  </si>
+  <si>
+    <t>{0: 181.38487044674423, 1: 100.671476865}</t>
+  </si>
+  <si>
+    <t>{0: 169.72059065744597, 1: 90.69381172886389}</t>
+  </si>
+  <si>
+    <t>{0: 136.525224635, 1: 61.8333139}</t>
+  </si>
+  <si>
+    <t>{0: 160.860786171771, 1: 44.698544659671}</t>
+  </si>
+  <si>
+    <t>curr_step_speed</t>
+  </si>
+  <si>
+    <t>{0: 15.10149825139535, 1: 9.497755142857143}</t>
+  </si>
+  <si>
+    <t>{0: 25.88649576575943, 1: 22.05276670995381}</t>
+  </si>
+  <si>
+    <t>{0: 3.67851365, 1: 3.8224361499999997}</t>
+  </si>
+  <si>
+    <t>{0: 5.45376433749, 1: 5.667143835989999}</t>
+  </si>
+  <si>
+    <t>cumm_step_calorie</t>
+  </si>
+  <si>
+    <t>{0: 142.38651273601164, 1: 67.23203601164286}</t>
+  </si>
+  <si>
+    <t>{0: 150.37264062266834, 1: 87.22799347205266}</t>
+  </si>
+  <si>
+    <t>{0: 97.4809534635, 1: 31.688641202}</t>
+  </si>
+  <si>
+    <t>{0: 131.5994616551601, 1: 22.6775993749263}</t>
+  </si>
+  <si>
+    <t>fats</t>
+  </si>
+  <si>
+    <t>{0: 0.8488372093023255, 1: 1.0}</t>
+  </si>
+  <si>
+    <t>{0: 0.847382709016626, 1: 0.5547001962252291}</t>
+  </si>
+  <si>
+    <t>{0: 1.0, 1: 1.0}</t>
+  </si>
+  <si>
+    <t>{0: 0.0, 1: 0.0}</t>
+  </si>
+  <si>
+    <t>cumm_step_count</t>
+  </si>
+  <si>
+    <t>{0: 2790.6511627906975, 1: 1335.142857142857}</t>
+  </si>
+  <si>
+    <t>{0: 2963.598598554057, 1: 1691.9862636805053}</t>
+  </si>
+  <si>
+    <t>{0: 2067.5, 1: 625.5}</t>
+  </si>
+  <si>
+    <t>{0: 2819.9051999999997, 1: 416.6106}</t>
+  </si>
+  <si>
+    <t>heart_rate</t>
+  </si>
+  <si>
+    <t>{0: 76.68703578510907, 1: 78.91280454042082}</t>
+  </si>
+  <si>
+    <t>{0: 9.001243887457901, 1: 7.17980969990852}</t>
+  </si>
+  <si>
+    <t>{0: 76.49932170542635, 1: 77.5826550387597}</t>
+  </si>
+  <si>
+    <t>{0: 8.40039436046512, 1: 8.747339999999998}</t>
+  </si>
+  <si>
+    <t>MeanBreathingTime</t>
+  </si>
+  <si>
+    <t>{0: 3.481115404968801, 1: 3.2492244975262836}</t>
+  </si>
+  <si>
+    <t>{0: 1.7051151144221162, 1: 0.987532598363854}</t>
+  </si>
+  <si>
+    <t>{0: 3.0936499999999993, 1: 2.8365}</t>
+  </si>
+  <si>
+    <t>{0: 0.8474129766666685, 1: 0.5659540384615384}</t>
+  </si>
+  <si>
+    <t>Consistency</t>
+  </si>
+  <si>
+    <t>{0: 0.7486328615429532, 1: 0.7005607927328394}</t>
+  </si>
+  <si>
+    <t>{0: 0.2131360350415756, 1: 0.2523623836841506}</t>
+  </si>
+  <si>
+    <t>{0: 0.8110455716575516, 1: 0.8175448598613219}</t>
+  </si>
+  <si>
+    <t>{0: 0.11630733709348871, 1: 0.15778783388103065}</t>
+  </si>
+  <si>
+    <t>sugars</t>
+  </si>
+  <si>
+    <t>{0: 1.069767441860465, 1: 1.0}</t>
+  </si>
+  <si>
+    <t>{0: 0.6649316227459003, 1: 0.5547001962252291}</t>
+  </si>
+  <si>
+    <t>past_day_fats</t>
+  </si>
+  <si>
+    <t>{0: 5.046511627906977, 1: 6.214285714285714}</t>
+  </si>
+  <si>
+    <t>{0: 4.236832825824126, 1: 4.854475673637068}</t>
+  </si>
+  <si>
+    <t>{0: 4.0, 1: 4.5}</t>
+  </si>
+  <si>
+    <t>{0: 2.9652, 1: 0.7413}</t>
+  </si>
+  <si>
+    <t>time_of_day</t>
+  </si>
+  <si>
+    <t>{0: 2.7906976744186047, 1: 3.0}</t>
+  </si>
+  <si>
+    <t>{0: 1.096693201452519, 1: 0.9607689228305231}</t>
+  </si>
+  <si>
+    <t>{0: 3.0, 1: 3.0}</t>
+  </si>
+  <si>
+    <t>{0: 1.4826, 1: 1.4826}</t>
+  </si>
+  <si>
+    <t>exercise_calorie</t>
+  </si>
+  <si>
+    <t>{0: 66.75322093023256, 1: 100.54478571428571}</t>
+  </si>
+  <si>
+    <t>{0: 132.1473966848161, 1: 146.8576955460775}</t>
+  </si>
+  <si>
+    <t>curr_step_count</t>
+  </si>
+  <si>
+    <t>{0: 262.3837209302326, 1: 87.78571428571429}</t>
+  </si>
+  <si>
+    <t>{0: 607.936087364543, 1: 152.80564758563716}</t>
+  </si>
+  <si>
+    <t>{0: 29.0, 1: 19.5}</t>
+  </si>
+  <si>
+    <t>{0: 42.9954, 1: 28.9107}</t>
+  </si>
+  <si>
+    <t>exercise_duration</t>
+  </si>
+  <si>
+    <t>{0: 351685.81395348837, 1: 548334.4285714285}</t>
+  </si>
+  <si>
+    <t>{0: 658054.049010557, 1: 755623.2229261755}</t>
+  </si>
+  <si>
+    <t>past_day_sugars</t>
+  </si>
+  <si>
+    <t>{0: 7.569767441860465, 1: 8.428571428571429}</t>
+  </si>
+  <si>
+    <t>{0: 8.374387700425931, 1: 11.105883996362438}</t>
+  </si>
+  <si>
+    <t>{0: 4.5, 1: 4.0}</t>
+  </si>
+  <si>
+    <t>{0: 2.2239, 1: 1.4826}</t>
+  </si>
+  <si>
+    <t>curr_step_calorie</t>
+  </si>
+  <si>
+    <t>{0: 13.395404053558137, 1: 4.380543109857142}</t>
+  </si>
+  <si>
+    <t>{0: 30.7943570031751, 1: 7.552849762807568}</t>
+  </si>
+  <si>
+    <t>{0: 1.639999961, 1: 1.135000003}</t>
+  </si>
+  <si>
+    <t>{0: 2.4314639421786, 1: 1.6827510044478}</t>
+  </si>
+  <si>
+    <t>curr_step_distance</t>
+  </si>
+  <si>
+    <t>{0: 199.7839289454651, 1: 66.66992370357143}</t>
+  </si>
+  <si>
+    <t>{0: 457.01183102669717, 1: 117.2467269560424}</t>
+  </si>
+  <si>
+    <t>{0: 23.43961545, 1: 16.195000150000002}</t>
+  </si>
+  <si>
+    <t>{0: 34.75157386617, 1: 24.010707222390003}</t>
+  </si>
+  <si>
+    <t>past_day_caffeine</t>
+  </si>
+  <si>
+    <t>{0: 1.7906976744186047, 1: 1.7142857142857142}</t>
+  </si>
+  <si>
+    <t>{0: 1.6529209729500247, 1: 1.3259870882635918}</t>
+  </si>
+  <si>
+    <t>{0: 2.0, 1: 1.0}</t>
+  </si>
+  <si>
     <t>caffeine</t>
   </si>
   <si>
@@ -66,300 +363,6 @@
   </si>
   <si>
     <t>{0: 0.6715846869844977, 1: 0.5135525910130955}</t>
-  </si>
-  <si>
-    <t>{0: 0.0, 1: 0.0}</t>
-  </si>
-  <si>
-    <t>fats</t>
-  </si>
-  <si>
-    <t>{0: 0.8488372093023255, 1: 1.0}</t>
-  </si>
-  <si>
-    <t>{0: 0.847382709016626, 1: 0.5547001962252291}</t>
-  </si>
-  <si>
-    <t>{0: 1.0, 1: 1.0}</t>
-  </si>
-  <si>
-    <t>sugars</t>
-  </si>
-  <si>
-    <t>{0: 1.069767441860465, 1: 1.0}</t>
-  </si>
-  <si>
-    <t>{0: 0.6649316227459003, 1: 0.5547001962252291}</t>
-  </si>
-  <si>
-    <t>MeanBreathingTime</t>
-  </si>
-  <si>
-    <t>{0: 3.481115404968801, 1: 3.2492244975262836}</t>
-  </si>
-  <si>
-    <t>{0: 1.7051151144221162, 1: 0.987532598363854}</t>
-  </si>
-  <si>
-    <t>{0: 3.0936499999999993, 1: 2.8365}</t>
-  </si>
-  <si>
-    <t>{0: 0.8474129766666685, 1: 0.5659540384615384}</t>
-  </si>
-  <si>
-    <t>Consistency</t>
-  </si>
-  <si>
-    <t>{0: 0.7486328615429532, 1: 0.7005607927328394}</t>
-  </si>
-  <si>
-    <t>{0: 0.2131360350415756, 1: 0.2523623836841506}</t>
-  </si>
-  <si>
-    <t>{0: 0.8110455716575516, 1: 0.8175448598613219}</t>
-  </si>
-  <si>
-    <t>{0: 0.11630733709348871, 1: 0.15778783388103065}</t>
-  </si>
-  <si>
-    <t>past_day_fats</t>
-  </si>
-  <si>
-    <t>{0: 5.046511627906977, 1: 6.214285714285714}</t>
-  </si>
-  <si>
-    <t>{0: 4.236832825824126, 1: 4.854475673637068}</t>
-  </si>
-  <si>
-    <t>{0: 4.0, 1: 4.5}</t>
-  </si>
-  <si>
-    <t>{0: 2.9652, 1: 0.7413}</t>
-  </si>
-  <si>
-    <t>past_day_sugars</t>
-  </si>
-  <si>
-    <t>{0: 7.569767441860465, 1: 8.428571428571429}</t>
-  </si>
-  <si>
-    <t>{0: 8.374387700425931, 1: 11.105883996362438}</t>
-  </si>
-  <si>
-    <t>{0: 4.5, 1: 4.0}</t>
-  </si>
-  <si>
-    <t>{0: 2.2239, 1: 1.4826}</t>
-  </si>
-  <si>
-    <t>past_day_caffeine</t>
-  </si>
-  <si>
-    <t>{0: 1.7906976744186047, 1: 1.7142857142857142}</t>
-  </si>
-  <si>
-    <t>{0: 1.6529209729500247, 1: 1.3259870882635918}</t>
-  </si>
-  <si>
-    <t>{0: 2.0, 1: 1.0}</t>
-  </si>
-  <si>
-    <t>heart_rate</t>
-  </si>
-  <si>
-    <t>{0: 76.68703578510907, 1: 78.91280454042082}</t>
-  </si>
-  <si>
-    <t>{0: 9.001243887457901, 1: 7.17980969990852}</t>
-  </si>
-  <si>
-    <t>{0: 76.49932170542635, 1: 77.5826550387597}</t>
-  </si>
-  <si>
-    <t>{0: 8.40039436046512, 1: 8.747339999999998}</t>
-  </si>
-  <si>
-    <t>ppg_std</t>
-  </si>
-  <si>
-    <t>{0: 144895.1541374223, 1: 180694.1595503829}</t>
-  </si>
-  <si>
-    <t>{0: 132374.97157583816, 1: 107879.52708056483}</t>
-  </si>
-  <si>
-    <t>{0: 95494.37235792716, 1: 151613.34293190698}</t>
-  </si>
-  <si>
-    <t>{0: 71328.03351750519, 1: 113676.25562711658}</t>
-  </si>
-  <si>
-    <t>curr_step_count</t>
-  </si>
-  <si>
-    <t>{0: 262.3837209302326, 1: 87.78571428571429}</t>
-  </si>
-  <si>
-    <t>{0: 607.936087364543, 1: 152.80564758563716}</t>
-  </si>
-  <si>
-    <t>{0: 29.0, 1: 19.5}</t>
-  </si>
-  <si>
-    <t>{0: 42.9954, 1: 28.9107}</t>
-  </si>
-  <si>
-    <t>curr_step_calorie</t>
-  </si>
-  <si>
-    <t>{0: 13.395404053558137, 1: 4.380543109857142}</t>
-  </si>
-  <si>
-    <t>{0: 30.7943570031751, 1: 7.552849762807568}</t>
-  </si>
-  <si>
-    <t>{0: 1.639999961, 1: 1.135000003}</t>
-  </si>
-  <si>
-    <t>{0: 2.4314639421786, 1: 1.6827510044478}</t>
-  </si>
-  <si>
-    <t>curr_step_speed</t>
-  </si>
-  <si>
-    <t>{0: 15.10149825139535, 1: 9.497755142857143}</t>
-  </si>
-  <si>
-    <t>{0: 25.88649576575943, 1: 22.05276670995381}</t>
-  </si>
-  <si>
-    <t>{0: 3.67851365, 1: 3.8224361499999997}</t>
-  </si>
-  <si>
-    <t>{0: 5.45376433749, 1: 5.667143835989999}</t>
-  </si>
-  <si>
-    <t>curr_step_distance</t>
-  </si>
-  <si>
-    <t>{0: 199.7839289454651, 1: 66.66992370357143}</t>
-  </si>
-  <si>
-    <t>{0: 457.01183102669717, 1: 117.2467269560424}</t>
-  </si>
-  <si>
-    <t>{0: 23.43961545, 1: 16.195000150000002}</t>
-  </si>
-  <si>
-    <t>{0: 34.75157386617, 1: 24.010707222390003}</t>
-  </si>
-  <si>
-    <t>cumm_step_count</t>
-  </si>
-  <si>
-    <t>{0: 2790.6511627906975, 1: 1335.142857142857}</t>
-  </si>
-  <si>
-    <t>{0: 2963.598598554057, 1: 1691.9862636805053}</t>
-  </si>
-  <si>
-    <t>{0: 2067.5, 1: 625.5}</t>
-  </si>
-  <si>
-    <t>{0: 2819.9051999999997, 1: 416.6106}</t>
-  </si>
-  <si>
-    <t>cumm_step_calorie</t>
-  </si>
-  <si>
-    <t>{0: 142.38651273601164, 1: 67.23203601164286}</t>
-  </si>
-  <si>
-    <t>{0: 150.37264062266834, 1: 87.22799347205266}</t>
-  </si>
-  <si>
-    <t>{0: 97.4809534635, 1: 31.688641202}</t>
-  </si>
-  <si>
-    <t>{0: 131.5994616551601, 1: 22.6775993749263}</t>
-  </si>
-  <si>
-    <t>cumm_step_speed</t>
-  </si>
-  <si>
-    <t>{0: 181.38487044674423, 1: 100.671476865}</t>
-  </si>
-  <si>
-    <t>{0: 169.72059065744597, 1: 90.69381172886389}</t>
-  </si>
-  <si>
-    <t>{0: 136.525224635, 1: 61.8333139}</t>
-  </si>
-  <si>
-    <t>{0: 160.860786171771, 1: 44.698544659671}</t>
-  </si>
-  <si>
-    <t>cumm_step_distance</t>
-  </si>
-  <si>
-    <t>{0: 2126.4325836626754, 1: 994.6574599785714}</t>
-  </si>
-  <si>
-    <t>{0: 2250.126647830915, 1: 1289.388057974536}</t>
-  </si>
-  <si>
-    <t>{0: 1535.981761385, 1: 464.135351065}</t>
-  </si>
-  <si>
-    <t>{0: 2081.1825957916767, 1: 343.5841717532699}</t>
-  </si>
-  <si>
-    <t>exercise_calorie</t>
-  </si>
-  <si>
-    <t>{0: 66.75322093023256, 1: 100.54478571428571}</t>
-  </si>
-  <si>
-    <t>{0: 132.1473966848161, 1: 146.8576955460775}</t>
-  </si>
-  <si>
-    <t>exercise_duration</t>
-  </si>
-  <si>
-    <t>{0: 351685.81395348837, 1: 548334.4285714285}</t>
-  </si>
-  <si>
-    <t>{0: 658054.049010557, 1: 755623.2229261755}</t>
-  </si>
-  <si>
-    <t>prev_night_sleep</t>
-  </si>
-  <si>
-    <t>{0: 5.184126347678875, 1: 5.792857142857143}</t>
-  </si>
-  <si>
-    <t>{0: 2.5056831230876324, 1: 2.7848008896716467}</t>
-  </si>
-  <si>
-    <t>{0: 5.366666666666666, 1: 6.433333333333334}</t>
-  </si>
-  <si>
-    <t>{0: 1.7544100000000002, 1: 4.991420000000001}</t>
-  </si>
-  <si>
-    <t>time_of_day</t>
-  </si>
-  <si>
-    <t>{0: 2.7906976744186047, 1: 3.0}</t>
-  </si>
-  <si>
-    <t>{0: 1.096693201452519, 1: 0.9607689228305231}</t>
-  </si>
-  <si>
-    <t>{0: 3.0, 1: 3.0}</t>
-  </si>
-  <si>
-    <t>{0: 1.4826, 1: 1.4826}</t>
   </si>
   <si>
     <t>rf</t>
@@ -427,9 +430,6 @@
   </si>
   <si>
     <t>f1_macro</t>
-  </si>
-  <si>
-    <t>rank</t>
   </si>
   <si>
     <t>Week 1 Mean-0</t>
@@ -919,10 +919,690 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>0.19101239593977951</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>0.13090927121131141</v>
+      </c>
+      <c r="I2">
+        <v>0.38837610339768031</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>9.7695447864175097E-2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3">
+        <v>4.9568665491823719E-2</v>
+      </c>
+      <c r="I3">
+        <v>0.29351585078507147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>0.1091798576456838</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4">
+        <v>0.1135220615145119</v>
+      </c>
+      <c r="I4">
+        <v>0.23754895814151561</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>7.8966329852069819E-2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5">
+        <v>7.2452511713595028E-2</v>
+      </c>
+      <c r="I5">
+        <v>0.2072727132535247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>0.1134503681707511</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6">
+        <v>0.18022148948686811</v>
+      </c>
+      <c r="I6">
+        <v>0.19440499846956369</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7">
+        <v>7.1028567618183616E-2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7">
+        <v>0.12135531852962329</v>
+      </c>
+      <c r="I7">
+        <v>0.14980155893836061</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8">
+        <v>5.1123597169858447E-2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8">
+        <v>9.3607793930636507E-2</v>
+      </c>
+      <c r="I8">
+        <v>0.12109348055618679</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9">
+        <v>4.9765892694098757E-2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9">
+        <v>0.11936226771272559</v>
+      </c>
+      <c r="I9">
+        <v>0.1057819905384499</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10">
+        <v>3.0836700052987651E-2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10">
+        <v>7.5237428913172727E-2</v>
+      </c>
+      <c r="I10">
+        <v>7.977782550947296E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11">
+        <v>5.4475379416150063E-2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11">
+        <v>0.31145599721066941</v>
+      </c>
+      <c r="I11">
+        <v>6.354537819490258E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12">
+        <v>5.5783595424406453E-2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12">
+        <v>0.43490132527774578</v>
+      </c>
+      <c r="I12">
+        <v>4.6447436011304508E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13">
+        <v>1.8557854692715509E-2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13">
+        <v>0.34533493093523288</v>
+      </c>
+      <c r="I13">
+        <v>1.973146304723726E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14">
+        <v>8.2139550546305191E-3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14">
+        <v>0.10171061856031829</v>
+      </c>
+      <c r="I14">
+        <v>1.8774009281989249E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15">
+        <v>1.4066058122390569E-2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15">
+        <v>0.27567398358778628</v>
+      </c>
+      <c r="I15">
+        <v>1.812462691535615E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16">
+        <v>8.2958348189748812E-3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16">
+        <v>0.1223535135491662</v>
+      </c>
+      <c r="I16">
+        <v>1.7428228028033638E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17">
+        <v>8.3805466953737317E-3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" t="s">
+        <v>83</v>
+      </c>
+      <c r="H17">
+        <v>0.18335127146586641</v>
+      </c>
+      <c r="I17">
+        <v>1.421635253724045E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18">
+        <v>5.3372841376782068E-3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18">
+        <v>8.9912594510532351E-2</v>
+      </c>
+      <c r="I18">
+        <v>1.2857075841549531E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19">
+        <v>1.7359874919124409E-2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19">
+        <v>0.4919880323744219</v>
+      </c>
+      <c r="I19">
+        <v>1.23133746823004E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20">
+        <v>4.7231526002886942E-3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" t="s">
+        <v>95</v>
+      </c>
+      <c r="G20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20">
+        <v>0.19113637773894929</v>
+      </c>
+      <c r="I20">
+        <v>7.8157221889767498E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21">
+        <v>4.7795512767224756E-3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" t="s">
+        <v>100</v>
+      </c>
+      <c r="G21" t="s">
+        <v>101</v>
+      </c>
+      <c r="H21">
+        <v>0.2097651736783579</v>
+      </c>
+      <c r="I21">
+        <v>7.4645435207758969E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="1">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22">
+        <v>5.6214499025874706E-3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" t="s">
+        <v>104</v>
+      </c>
+      <c r="F22" t="s">
+        <v>105</v>
+      </c>
+      <c r="G22" t="s">
+        <v>91</v>
+      </c>
+      <c r="H22">
+        <v>0.47766921688544711</v>
+      </c>
+      <c r="I22">
+        <v>4.1533340626019634E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="1">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23">
+        <v>1.3463059313692509E-3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23">
+        <v>0.2201086960157547</v>
+      </c>
+      <c r="I23">
+        <v>2.0378141384183482E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
@@ -954,22 +1634,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="C2">
         <v>5.0734126588620294E-3</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H2">
         <v>0.2201086960157547</v>
@@ -980,22 +1660,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>2.7723849306500559E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H3">
         <v>9.3607793930636507E-2</v>
@@ -1006,22 +1686,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="C4">
         <v>3.6196805584956629E-4</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H4">
         <v>0.34533493093523288</v>
@@ -1032,22 +1712,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="C5">
         <v>5.7072592355271623E-2</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="H5">
         <v>0.31145599721066941</v>
@@ -1058,22 +1738,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="C6">
         <v>3.5056617969544838E-2</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="H6">
         <v>0.43490132527774578</v>
@@ -1084,22 +1764,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="C7">
         <v>1.5707887905661449E-2</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="H7">
         <v>0.10171061856031829</v>
@@ -1110,22 +1790,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="C8">
         <v>9.7727333575195197E-3</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="H8">
         <v>0.4919880323744219</v>
@@ -1136,22 +1816,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="C9">
         <v>1.167553788066869E-2</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="H9">
         <v>0.47766921688544711</v>
@@ -1162,22 +1842,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C10">
         <v>4.7024668758004519E-2</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="H10">
         <v>7.5237428913172727E-2</v>
@@ -1188,22 +1868,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>0.12986696513964491</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="H11">
         <v>4.9568665491823719E-2</v>
@@ -1214,22 +1894,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="C12">
         <v>1.941906962794231E-2</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="G12" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="H12">
         <v>0.18335127146586641</v>
@@ -1240,22 +1920,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="C13">
         <v>1.666855784552319E-2</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="G13" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="H13">
         <v>0.19113637773894929</v>
@@ -1266,22 +1946,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>8.1234857091963306E-2</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="G14" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="H14">
         <v>0.18022148948686811</v>
@@ -1292,22 +1972,22 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="C15">
         <v>2.316114010870951E-2</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="F15" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="G15" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="H15">
         <v>0.2097651736783579</v>
@@ -1318,22 +1998,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="C16">
         <v>7.1449430642179124E-2</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="F16" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="G16" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="H16">
         <v>0.11936226771272559</v>
@@ -1344,22 +2024,22 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="C17">
         <v>6.9518107957118686E-2</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="G17" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="H17">
         <v>0.12135531852962329</v>
@@ -1370,22 +2050,22 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>7.0922219575473316E-2</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="G18" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="H18">
         <v>7.2452511713595028E-2</v>
@@ -1396,22 +2076,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>0.15681447915922289</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="G19" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="H19">
         <v>0.1135220615145119</v>
@@ -1422,22 +2102,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C20">
         <v>8.3250665560043041E-3</v>
       </c>
       <c r="D20" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="E20" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G20" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H20">
         <v>0.1223535135491662</v>
@@ -1448,22 +2128,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C21">
         <v>3.4359816011006838E-3</v>
       </c>
       <c r="D21" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E21" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G21" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H21">
         <v>8.9912594510532351E-2</v>
@@ -1474,22 +2154,22 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>8</v>
       </c>
       <c r="C22">
         <v>0.1546108151926058</v>
       </c>
       <c r="D22" t="s">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>101</v>
+        <v>11</v>
       </c>
       <c r="G22" t="s">
-        <v>102</v>
+        <v>12</v>
       </c>
       <c r="H22">
         <v>0.13090927121131141</v>
@@ -1500,22 +2180,22 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="C23">
         <v>1.0055505630479539E-2</v>
       </c>
       <c r="D23" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="E23" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="F23" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="G23" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="H23">
         <v>0.27567398358778628</v>
@@ -1526,7 +2206,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
@@ -1562,22 +2242,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="C2">
         <v>1.3463059313692509E-3</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H2">
         <v>0.2201086960157547</v>
@@ -1588,22 +2268,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>5.1123597169858447E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H3">
         <v>9.3607793930636507E-2</v>
@@ -1614,22 +2294,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="C4">
         <v>1.8557854692715509E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H4">
         <v>0.34533493093523288</v>
@@ -1640,22 +2320,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="C5">
         <v>5.4475379416150063E-2</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="H5">
         <v>0.31145599721066941</v>
@@ -1666,22 +2346,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="C6">
         <v>5.5783595424406453E-2</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="H6">
         <v>0.43490132527774578</v>
@@ -1692,22 +2372,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="C7">
         <v>8.2139550546305191E-3</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="H7">
         <v>0.10171061856031829</v>
@@ -1718,22 +2398,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="C8">
         <v>1.7359874919124409E-2</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="H8">
         <v>0.4919880323744219</v>
@@ -1744,22 +2424,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="C9">
         <v>5.6214499025874706E-3</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="H9">
         <v>0.47766921688544711</v>
@@ -1770,22 +2450,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C10">
         <v>3.0836700052987651E-2</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="H10">
         <v>7.5237428913172727E-2</v>
@@ -1796,22 +2476,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>9.7695447864175097E-2</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="H11">
         <v>4.9568665491823719E-2</v>
@@ -1822,22 +2502,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="C12">
         <v>8.3805466953737317E-3</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="G12" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="H12">
         <v>0.18335127146586641</v>
@@ -1848,22 +2528,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="C13">
         <v>4.7231526002886942E-3</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="G13" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="H13">
         <v>0.19113637773894929</v>
@@ -1874,22 +2554,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>0.1134503681707511</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="G14" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="H14">
         <v>0.18022148948686811</v>
@@ -1900,22 +2580,22 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="C15">
         <v>4.7795512767224756E-3</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="F15" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="G15" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="H15">
         <v>0.2097651736783579</v>
@@ -1926,22 +2606,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="C16">
         <v>4.9765892694098757E-2</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="F16" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="G16" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="H16">
         <v>0.11936226771272559</v>
@@ -1952,22 +2632,22 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="C17">
         <v>7.1028567618183616E-2</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="G17" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="H17">
         <v>0.12135531852962329</v>
@@ -1978,22 +2658,22 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>7.8966329852069819E-2</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="G18" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="H18">
         <v>7.2452511713595028E-2</v>
@@ -2004,22 +2684,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>0.1091798576456838</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="G19" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="H19">
         <v>0.1135220615145119</v>
@@ -2030,22 +2710,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C20">
         <v>8.2958348189748812E-3</v>
       </c>
       <c r="D20" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="E20" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G20" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H20">
         <v>0.1223535135491662</v>
@@ -2056,22 +2736,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C21">
         <v>5.3372841376782068E-3</v>
       </c>
       <c r="D21" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E21" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G21" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H21">
         <v>8.9912594510532351E-2</v>
@@ -2082,22 +2762,22 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>8</v>
       </c>
       <c r="C22">
         <v>0.19101239593977951</v>
       </c>
       <c r="D22" t="s">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>101</v>
+        <v>11</v>
       </c>
       <c r="G22" t="s">
-        <v>102</v>
+        <v>12</v>
       </c>
       <c r="H22">
         <v>0.13090927121131141</v>
@@ -2108,22 +2788,22 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="C23">
         <v>1.4066058122390569E-2</v>
       </c>
       <c r="D23" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="E23" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="F23" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="G23" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="H23">
         <v>0.27567398358778628</v>
@@ -2134,7 +2814,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
@@ -2170,22 +2850,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="C2">
         <v>8.3333333333333339E-4</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H2">
         <v>0.2201086960157547</v>
@@ -2196,22 +2876,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>1.403333333333333E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H3">
         <v>9.3607793930636507E-2</v>
@@ -2222,22 +2902,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="C4">
         <v>2.47E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H4">
         <v>0.34533493093523288</v>
@@ -2248,22 +2928,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="C5">
         <v>0.15736666666666671</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="H5">
         <v>0.31145599721066941</v>
@@ -2274,22 +2954,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="C6">
         <v>4.3600000000000007E-2</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="H6">
         <v>0.43490132527774578</v>
@@ -2300,22 +2980,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="C7">
         <v>6.0333333333333341E-3</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="H7">
         <v>0.10171061856031829</v>
@@ -2326,22 +3006,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="C8">
         <v>1.493333333333333E-2</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="H8">
         <v>0.4919880323744219</v>
@@ -2352,22 +3032,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="C9">
         <v>5.0999999999999986E-3</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="H9">
         <v>0.47766921688544711</v>
@@ -2378,22 +3058,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C10">
         <v>5.1633333333333337E-2</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="H10">
         <v>7.5237428913172727E-2</v>
@@ -2404,22 +3084,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>4.3933333333333331E-2</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="H11">
         <v>4.9568665491823719E-2</v>
@@ -2430,22 +3110,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="C12">
         <v>6.2433333333333327E-2</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="G12" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="H12">
         <v>0.18335127146586641</v>
@@ -2456,22 +3136,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="C13">
         <v>2.76E-2</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="G13" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="H13">
         <v>0.19113637773894929</v>
@@ -2482,22 +3162,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>0.15583333333333341</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="G14" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="H14">
         <v>0.18022148948686811</v>
@@ -2508,22 +3188,22 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="C15">
         <v>1.26E-2</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="F15" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="G15" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="H15">
         <v>0.2097651736783579</v>
@@ -2534,22 +3214,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="C16">
         <v>4.9466666666666659E-2</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="F16" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="G16" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="H16">
         <v>0.11936226771272559</v>
@@ -2560,22 +3240,22 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="C17">
         <v>8.0933333333333329E-2</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="G17" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="H17">
         <v>0.12135531852962329</v>
@@ -2586,22 +3266,22 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>3.6033333333333327E-2</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="G18" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="H18">
         <v>7.2452511713595028E-2</v>
@@ -2612,22 +3292,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>7.9500000000000001E-2</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="G19" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="H19">
         <v>0.1135220615145119</v>
@@ -2638,22 +3318,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C20">
         <v>1.1033333333333331E-2</v>
       </c>
       <c r="D20" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="E20" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G20" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H20">
         <v>0.1223535135491662</v>
@@ -2664,22 +3344,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C21">
         <v>6.4666666666666666E-3</v>
       </c>
       <c r="D21" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E21" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G21" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H21">
         <v>8.9912594510532351E-2</v>
@@ -2690,22 +3370,22 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>8</v>
       </c>
       <c r="C22">
         <v>0.1128333333333333</v>
       </c>
       <c r="D22" t="s">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>101</v>
+        <v>11</v>
       </c>
       <c r="G22" t="s">
-        <v>102</v>
+        <v>12</v>
       </c>
       <c r="H22">
         <v>0.13090927121131141</v>
@@ -2716,22 +3396,22 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="C23">
         <v>3.0999999999999999E-3</v>
       </c>
       <c r="D23" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="E23" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="F23" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="G23" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="H23">
         <v>0.27567398358778628</v>
@@ -2742,7 +3422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
@@ -2778,22 +3458,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="C2">
         <v>2.0662022230112761E-2</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H2">
         <v>0.2201086960157547</v>
@@ -2804,22 +3484,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>8.3947152592104453E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H3">
         <v>9.3607793930636507E-2</v>
@@ -2830,22 +3510,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="C4">
         <v>1.419883126874253E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H4">
         <v>0.34533493093523288</v>
@@ -2856,22 +3536,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="C5">
         <v>8.5234349204139262E-2</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="H5">
         <v>0.31145599721066941</v>
@@ -2882,22 +3562,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="C6">
         <v>7.7219602271848806E-2</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="H6">
         <v>0.43490132527774578</v>
@@ -2908,22 +3588,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="C7">
         <v>3.2841641962663641E-2</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="H7">
         <v>0.10171061856031829</v>
@@ -2934,22 +3614,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="C8">
         <v>4.0109817821356412E-2</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="H8">
         <v>0.4919880323744219</v>
@@ -2960,22 +3640,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="C9">
         <v>4.0804454265909153E-2</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="H9">
         <v>0.47766921688544711</v>
@@ -2986,22 +3666,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C10">
         <v>5.0770240646480343E-2</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="H10">
         <v>7.5237428913172727E-2</v>
@@ -3012,22 +3692,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>6.1894406279865533E-2</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="H11">
         <v>4.9568665491823719E-2</v>
@@ -3038,22 +3718,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="C12">
         <v>3.708179431023443E-2</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="G12" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="H12">
         <v>0.18335127146586641</v>
@@ -3064,22 +3744,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="C13">
         <v>3.6496639562221607E-2</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="G13" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="H13">
         <v>0.19113637773894929</v>
@@ -3090,22 +3770,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>5.4695182207421568E-2</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="G14" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="H14">
         <v>0.18022148948686811</v>
@@ -3116,22 +3796,22 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="C15">
         <v>3.828784430741948E-2</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="F15" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="G15" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="H15">
         <v>0.2097651736783579</v>
@@ -3142,22 +3822,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="C16">
         <v>5.7315861287671993E-2</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="F16" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="G16" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="H16">
         <v>0.11936226771272559</v>
@@ -3168,22 +3848,22 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="C17">
         <v>5.833335276559632E-2</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="G17" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="H17">
         <v>0.12135531852962329</v>
@@ -3194,22 +3874,22 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>6.9437051362169558E-2</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="G18" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="H18">
         <v>7.2452511713595028E-2</v>
@@ -3220,22 +3900,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>6.001779696770565E-2</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="G19" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="H19">
         <v>0.1135220615145119</v>
@@ -3246,22 +3926,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C20">
         <v>1.7470670737425489E-2</v>
       </c>
       <c r="D20" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="E20" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G20" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H20">
         <v>0.1223535135491662</v>
@@ -3272,22 +3952,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C21">
         <v>1.561248623786704E-2</v>
       </c>
       <c r="D21" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E21" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G21" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H21">
         <v>8.9912594510532351E-2</v>
@@ -3298,22 +3978,22 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>8</v>
       </c>
       <c r="C22">
         <v>9.3556216513317303E-2</v>
       </c>
       <c r="D22" t="s">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>101</v>
+        <v>11</v>
       </c>
       <c r="G22" t="s">
-        <v>102</v>
+        <v>12</v>
       </c>
       <c r="H22">
         <v>0.13090927121131141</v>
@@ -3324,22 +4004,22 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="C23">
         <v>2.9565022530620679E-2</v>
       </c>
       <c r="D23" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="E23" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="F23" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="G23" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="H23">
         <v>0.27567398358778628</v>
@@ -3350,7 +4030,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -3360,56 +4040,56 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B3">
         <v>0.82889237199582022</v>
@@ -3435,7 +4115,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B4">
         <v>0.58456486042692946</v>
@@ -3461,7 +4141,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B5">
         <v>0.65024777099080511</v>
@@ -3487,7 +4167,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B6">
         <v>9.9067599067599058E-2</v>
@@ -3513,7 +4193,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B7">
         <v>0.3666666666666667</v>
@@ -3539,7 +4219,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B8">
         <v>0.15340501792114691</v>
@@ -3565,7 +4245,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B9">
         <v>0.82451379466304842</v>
@@ -3591,7 +4271,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B10">
         <v>0.90693756199901943</v>
@@ -3617,7 +4297,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B11">
         <v>0.82451379466304842</v>
@@ -3643,7 +4323,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B12">
         <v>0.56298276886512177</v>
@@ -3669,7 +4349,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B13">
         <v>0.72822718477798698</v>
@@ -3695,7 +4375,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B14">
         <v>0.56298276886512177</v>
@@ -3721,7 +4401,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B15">
         <v>0.40182639445597601</v>
@@ -3743,683 +4423,6 @@
       </c>
       <c r="H15">
         <v>0.4282872680235475</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2">
-        <v>0.19101239593977951</v>
-      </c>
-      <c r="D2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2">
-        <v>0.13090927121131141</v>
-      </c>
-      <c r="I2">
-        <v>0.38837610339768031</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3">
-        <v>9.7695447864175097E-2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3">
-        <v>4.9568665491823719E-2</v>
-      </c>
-      <c r="I3">
-        <v>0.29351585078507147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4">
-        <v>0.1091798576456838</v>
-      </c>
-      <c r="D4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G4" t="s">
-        <v>91</v>
-      </c>
-      <c r="H4">
-        <v>0.1135220615145119</v>
-      </c>
-      <c r="I4">
-        <v>0.23754895814151561</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="1">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5">
-        <v>7.8966329852069819E-2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G5" t="s">
-        <v>86</v>
-      </c>
-      <c r="H5">
-        <v>7.2452511713595028E-2</v>
-      </c>
-      <c r="I5">
-        <v>0.2072727132535247</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="1">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6">
-        <v>0.1134503681707511</v>
-      </c>
-      <c r="D6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6">
-        <v>0.18022148948686811</v>
-      </c>
-      <c r="I6">
-        <v>0.19440499846956369</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="1">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7">
-        <v>7.1028567618183616E-2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G7" t="s">
-        <v>81</v>
-      </c>
-      <c r="H7">
-        <v>0.12135531852962329</v>
-      </c>
-      <c r="I7">
-        <v>0.14980155893836061</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8">
-        <v>5.1123597169858447E-2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8">
-        <v>9.3607793930636507E-2</v>
-      </c>
-      <c r="I8">
-        <v>0.12109348055618679</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9">
-        <v>4.9765892694098757E-2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" t="s">
-        <v>75</v>
-      </c>
-      <c r="G9" t="s">
-        <v>76</v>
-      </c>
-      <c r="H9">
-        <v>0.11936226771272559</v>
-      </c>
-      <c r="I9">
-        <v>0.1057819905384499</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10">
-        <v>3.0836700052987651E-2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10">
-        <v>7.5237428913172727E-2</v>
-      </c>
-      <c r="I10">
-        <v>7.977782550947296E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="1">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11">
-        <v>5.4475379416150063E-2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11">
-        <v>0.31145599721066941</v>
-      </c>
-      <c r="I11">
-        <v>6.354537819490258E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="1">
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12">
-        <v>5.5783595424406453E-2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12">
-        <v>0.43490132527774578</v>
-      </c>
-      <c r="I12">
-        <v>4.6447436011304508E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="1">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>1.8557854692715509E-2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13">
-        <v>0.34533493093523288</v>
-      </c>
-      <c r="I13">
-        <v>1.973146304723726E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="1">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14">
-        <v>8.2139550546305191E-3</v>
-      </c>
-      <c r="D14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14">
-        <v>0.10171061856031829</v>
-      </c>
-      <c r="I14">
-        <v>1.8774009281989249E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="1">
-        <v>21</v>
-      </c>
-      <c r="B15" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15">
-        <v>1.4066058122390569E-2</v>
-      </c>
-      <c r="D15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E15" t="s">
-        <v>105</v>
-      </c>
-      <c r="F15" t="s">
-        <v>106</v>
-      </c>
-      <c r="G15" t="s">
-        <v>107</v>
-      </c>
-      <c r="H15">
-        <v>0.27567398358778628</v>
-      </c>
-      <c r="I15">
-        <v>1.812462691535615E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="1">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C16">
-        <v>8.2958348189748812E-3</v>
-      </c>
-      <c r="D16" t="s">
-        <v>93</v>
-      </c>
-      <c r="E16" t="s">
-        <v>94</v>
-      </c>
-      <c r="F16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16">
-        <v>0.1223535135491662</v>
-      </c>
-      <c r="I16">
-        <v>1.7428228028033638E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="1">
-        <v>10</v>
-      </c>
-      <c r="B17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17">
-        <v>8.3805466953737317E-3</v>
-      </c>
-      <c r="D17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" t="s">
-        <v>56</v>
-      </c>
-      <c r="H17">
-        <v>0.18335127146586641</v>
-      </c>
-      <c r="I17">
-        <v>1.421635253724045E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="1">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>95</v>
-      </c>
-      <c r="C18">
-        <v>5.3372841376782068E-3</v>
-      </c>
-      <c r="D18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E18" t="s">
-        <v>97</v>
-      </c>
-      <c r="F18" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18">
-        <v>8.9912594510532351E-2</v>
-      </c>
-      <c r="I18">
-        <v>1.2857075841549531E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="1">
-        <v>6</v>
-      </c>
-      <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19">
-        <v>1.7359874919124409E-2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19" t="s">
-        <v>37</v>
-      </c>
-      <c r="H19">
-        <v>0.4919880323744219</v>
-      </c>
-      <c r="I19">
-        <v>1.23133746823004E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="1">
-        <v>11</v>
-      </c>
-      <c r="B20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20">
-        <v>4.7231526002886942E-3</v>
-      </c>
-      <c r="D20" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" t="s">
-        <v>59</v>
-      </c>
-      <c r="F20" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" t="s">
-        <v>61</v>
-      </c>
-      <c r="H20">
-        <v>0.19113637773894929</v>
-      </c>
-      <c r="I20">
-        <v>7.8157221889767498E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="1">
-        <v>13</v>
-      </c>
-      <c r="B21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21">
-        <v>4.7795512767224756E-3</v>
-      </c>
-      <c r="D21" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F21" t="s">
-        <v>70</v>
-      </c>
-      <c r="G21" t="s">
-        <v>71</v>
-      </c>
-      <c r="H21">
-        <v>0.2097651736783579</v>
-      </c>
-      <c r="I21">
-        <v>7.4645435207758969E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="1">
-        <v>7</v>
-      </c>
-      <c r="B22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22">
-        <v>5.6214499025874706E-3</v>
-      </c>
-      <c r="D22" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" t="s">
-        <v>41</v>
-      </c>
-      <c r="G22" t="s">
-        <v>37</v>
-      </c>
-      <c r="H22">
-        <v>0.47766921688544711</v>
-      </c>
-      <c r="I22">
-        <v>4.1533340626019634E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="1">
-        <v>0</v>
-      </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23">
-        <v>1.3463059313692509E-3</v>
-      </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23">
-        <v>0.2201086960157547</v>
-      </c>
-      <c r="I23">
-        <v>2.0378141384183482E-3</v>
       </c>
     </row>
   </sheetData>
@@ -4434,6 +4437,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:38">
       <c r="B1" s="1" t="s">
@@ -4545,12 +4551,12 @@
         <v>166</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>130</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:38">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>5.2693486590038336</v>
@@ -4666,7 +4672,7 @@
     </row>
     <row r="3" spans="1:38">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>253055.41648525489</v>
@@ -4782,7 +4788,7 @@
     </row>
     <row r="4" spans="1:38">
       <c r="A4" s="1" t="s">
-        <v>87</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>667.79999747500005</v>
@@ -4898,7 +4904,7 @@
     </row>
     <row r="5" spans="1:38">
       <c r="A5" s="1" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="B5">
         <v>93.060464400000001</v>
@@ -5014,7 +5020,7 @@
     </row>
     <row r="6" spans="1:38">
       <c r="A6" s="1" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -5130,7 +5136,7 @@
     </row>
     <row r="7" spans="1:38">
       <c r="A7" s="1" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="B7">
         <v>43.639995567</v>
@@ -5246,7 +5252,7 @@
     </row>
     <row r="8" spans="1:38">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5359,7 +5365,7 @@
     </row>
     <row r="9" spans="1:38">
       <c r="A9" s="1" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="B9">
         <v>869.5</v>
@@ -5475,7 +5481,7 @@
     </row>
     <row r="10" spans="1:38">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B10">
         <v>81.233333333333334</v>
@@ -5591,7 +5597,7 @@
     </row>
     <row r="11" spans="1:38">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="B11">
         <v>3.4094364500745362</v>
@@ -5707,7 +5713,7 @@
     </row>
     <row r="12" spans="1:38">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="B12">
         <v>0.83286915114403115</v>
@@ -5823,7 +5829,7 @@
     </row>
     <row r="13" spans="1:38">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -5936,7 +5942,7 @@
     </row>
     <row r="14" spans="1:38">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="B14">
         <v>4.5</v>
@@ -6052,7 +6058,7 @@
     </row>
     <row r="15" spans="1:38">
       <c r="A15" s="1" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -6168,7 +6174,7 @@
     </row>
     <row r="16" spans="1:38">
       <c r="A16" s="1" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -6284,7 +6290,7 @@
     </row>
     <row r="17" spans="1:38">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -6400,7 +6406,7 @@
     </row>
     <row r="18" spans="1:38">
       <c r="A18" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -6516,7 +6522,7 @@
     </row>
     <row r="19" spans="1:38">
       <c r="A19" s="1" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="B19">
         <v>4.5</v>
@@ -6632,7 +6638,7 @@
     </row>
     <row r="20" spans="1:38">
       <c r="A20" s="1" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -6748,7 +6754,7 @@
     </row>
     <row r="21" spans="1:38">
       <c r="A21" s="1" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -6864,7 +6870,7 @@
     </row>
     <row r="22" spans="1:38">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -6980,7 +6986,7 @@
     </row>
     <row r="23" spans="1:38">
       <c r="A23" s="1" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="B23">
         <v>0</v>

</xml_diff>